<commit_message>
Deleted old data, add new one data
</commit_message>
<xml_diff>
--- a/UIAotomation/src/main/java/uiAutomation/data/TestData.xlsx
+++ b/UIAotomation/src/main/java/uiAutomation/data/TestData.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="5565"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>UserName</t>
   </si>
@@ -28,13 +27,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Grey</t>
-  </si>
-  <si>
-    <t>Stephen</t>
-  </si>
-  <si>
-    <t>Stan</t>
+    <t>Victor</t>
   </si>
 </sst>
 </file>
@@ -352,15 +345,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -376,23 +370,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>8910</v>
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>